<commit_message>
py-spider --version: 4 multi-thread & automatic-run
</commit_message>
<xml_diff>
--- a/filtered_data/final_result/final_result.xlsx
+++ b/filtered_data/final_result/final_result.xlsx
@@ -389,12 +389,6 @@
     <t>诺维信一日斩获两项创新殊荣：生物技术推进可持续发展</t>
   </si>
   <si>
-    <t>http://mp.weixin.qq.com/s?__biz=MzA3OTI0OTk3OQ==&amp;mid=206606084&amp;idx=1&amp;sn=0d817888d2390a9d83ec57af10b639ce&amp;chksm=161278502165f14684415c538fb0e20c61df3ef332dcd3fed3f83b799803c0a3849dd33b7cae#rd</t>
-  </si>
-  <si>
-    <t>点击上方蓝色字体关注诺维信生物科技博览~【2015年7月22日，中国北京】全球生物解决方案领先者诺维信公司在今天举行的第四届中国财经峰会以及2015关注气候中国峰会上分别荣获 “最佳企业创新奖” 和 “中国绿色技术创新成果” 两大殊荣。 作为引领生物创新的世界先导，诺维信始终围绕可持续发展议题，不断推出改变生活的创新产品和解决方案，用生物技术为中国及世界的可持续发展做出非凡贡献。权威评定，成就多项殊荣中国财经峰会是经济领域最具影响力的思想盛会之一，诺维信经众多权威专家评定，最终凭借卓越的创新能力，脱颖而出摘得“最佳企业创新” 桂冠。该项殊荣是对诺维信始终秉承经营业绩、环境表现和社会责任并举的 ‘三重底线’ 的最佳表彰。中国财经峰会组委会表示：“ 诺维信坚持生物创新，不断提供可持续发展的解决方案，帮助客户使用更少原料、生产更多产品，减少对世界资源的消耗，是经济新常态下企业创新的典范。”同日，在京举行的另一以“行动的力量” 为主题的2015关注气候中国峰会，旨在彰显中国企业在绿色低碳发展领域的努力及成效。力求通过国际对话、专家研判以及思想碰撞等多角度、全方位展现中国企业在关注气候、促进生态文明、实现可持续发展方面的扎实行动和成功经验，向世界传递来自中国典范企业、区域的声音。诺维信同时荣登“中国绿色技术创新成果” 榜单，充分证明其绿色创新技术为中国行业和社会带来突出影响。诺维信亚太区总裁戴彤于当日分别出席两项颁奖活动并表示：今天问鼎双料嘉奖，反映了中国公众对诺维信公司的高度赞誉和认可，我们感到十分荣幸和欣慰。一直以来，创新就是诺维信的企业基因，以生物创新带动绿色可持续发展已成为诺维信人的共识，为我们使命所在。在诺维信的不断努力下，仅二代纤维素燃料乙醇一个领域，每年就可在生产过程中实现碳减排近3万吨； 2014年，诺维信生物技术的各项应用共为全球工业生产减少了约6000万吨二氧化碳排放，相当于2500万辆小汽车的年排放量。未来，诺维信将继续积极倡导并有效推动生态工业、农业和循环经济；更加植根中国发展，成为中国可持续发展进程中最值得信赖的重要战略合作伙伴。”持续创新，推动可持续发展诺维信强调经济、社会、环境在未来可持续业务增长中创造价值和贡献。诺维信的产品生命周期评估显示，酶的应用可显著节约原材料、化学品、能耗并提高质量。诺维信始终坚持创新，不断在洗涤、食品饮料、生物燃料、农业及饲料、微生物及生物制药等多个领域实现技术突破，成功运用生物科技实现降低洗衣温度、提升生产能效、提高农业产量和减少化学品添加，推进可持续发展的健康生活方式。近日，诺维信联手立白在中国发布国内首款攻克生物酶在洗衣液中应用难题的新品——永维酶洗衣液，助力合作伙伴以更绿色的产品开拓中高端洗衣液市场。面对人口不断增长致使粮食与食品需求激增的现状，诺维信积极研发并与合作伙伴达成农业联盟，用生物技术克服现行化学肥料和化学农药对生态环境的污染，同时降低成本、改善农作物品质等使种植业步入良态循环，长效增产。今天人们正孜孜不倦地寻求可再生能源的替代能源，由诺维信最新推出的Eversa®，是市场上第一个利用废油来生产生物柴油的酶制剂解决方案。与此同时，诺维信的Cellic® 作为纤维素乙醇产生过程中必不可少的催化剂，它的问世让农业废弃物从环境、大气污染源之一，变成输送未来清洁能源的原料。到2020年，诺维信全球还计划推出10项改变生活的革命性创新产品，实现二氧化碳减排1亿吨的重大目标。诺维信的愿景就是在更繁荣的经济，更清洁的能源和更美好的生活之间实现和谐与统一。长按下方二维码，选择“识别图中二维码”，了解诺维信中国运营业务，领略生物技术的魅力，更多礼品等待您。</t>
-  </si>
-  <si>
     <t>世界人口日|如何供养全球70亿人口？</t>
   </si>
   <si>
@@ -547,6 +541,14 @@
   </si>
   <si>
     <t>http://mp.weixin.qq.com/s?__biz=MzA3OTI0OTk3OQ==&amp;mid=2650316146&amp;idx=1&amp;sn=c3c210756e8af59cdb802f93c10d5170&amp;chksm=87ba6a26b0cde330659198aaee1276c04b2710b5699bb46b14e140b8a20bed56bde45e3ab7dc#rd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://mp.weixin.qq.com/s?__biz=MzA3OTI0OTk3OQ==&amp;mid=206606084&amp;idx=1&amp;sn=0d817888d2390a9d83ec57af10b639ce&amp;chksm=161278502165f14684415c538fb0e20c61df3ef332dcd3fed3f83b799803c0a3849dd33b7cae#rd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击上方蓝色字体关注诺维信生物科技博览~【2015年7月22日，中国北京】全球生物解决方案领先者诺维信公司在今天举行的第四届中国财经峰会以及2015关注气候中国峰会上分别荣获 “最佳企业创新奖” 和 “中国绿色技术创新成果” 两大殊荣。 作为引领生物创新的世界先导，诺维信始终围绕可持续发展议题，不断推出改变生活的创新产品和解决方案，用生物技术为中国及世界的可持续发展做出非凡贡献。权威评定，成就多项殊荣中国财经峰会是经济领域最具影响力的思想盛会之一，诺维信经众多权威专家评定，最终凭借卓越的创新能力，脱颖而出摘得“最佳企业创新” 桂冠。该项殊荣是对诺维信始终秉承经营业绩、环境表现和社会责任并举的 ‘三重底线’ 的最佳表彰。中国财经峰会组委会表示：“ 诺维信坚持生物创新，不断提供可持续发展的解决方案，帮助客户使用更少原料、生产更多产品，减少对世界资源的消耗，是经济新常态下企业创新的典范。”同日，在京举行的另一以“行动的力量” 为主题的2015关注气候中国峰会，旨在彰显中国企业在绿色低碳发展领域的努力及成效。力求通过国际对话、专家研判以及思想碰撞等多角度、全方位展现中国企业在关注气候、促进生态文明、实现可持续发展方面的扎实行动和成功经验，向世界传递来自中国典范企业、区域的声音。诺维信同时荣登“中国绿色技术创新成果” 榜单，充分证明其绿色创新技术为中国行业和社会带来突出影响。诺维信亚太区总裁戴彤于当日分别出席两项颁奖活动并表示：今天问鼎双料嘉奖，反映了中国公众对诺维信公司的高度赞誉和认可，我们感到十分荣幸和欣慰。一直以来，创新就是诺维信的企业基因，以生物创新带动绿色可持续发展已成为诺维信人的共识，为我们使命所在。在诺维信的不断努力下，仅二代纤维素燃料乙醇一个领域，每年就可在生产过程中实现碳减排近3万吨； 2014年，诺维信生物技术的各项应用共为全球工业生产减少了约6000万吨二氧化碳排放，相当于2500万辆小汽车的年排放量。未来，诺维信将继续积极倡导并有效推动生态工业、农业和循环经济；更加植根中国发展，成为中国可持续发展进程中最值得信赖的重要战略合作伙伴。”持续创新，推动可持续发展诺维信强调经济、社会、环境在未来可持续业务增长中创造价值和贡献。诺维信的产品生命周期评估显示，酶的应用可显著节约原材料、化学品、能耗并提高质量。诺维信始终坚持创新，不断在洗涤、食品饮料、生物燃料、农业及饲料、微生物及生物制药等多个领域实现技术突破，成功运用生物科技实现降低洗衣温度、提升生产能效、提高农业产量和减少化学品添加，推进可持续发展的健康生活方式。近日，诺维信联手立白在中国发布国内首款攻克生物酶在洗衣液中应用难题的新品——永维酶洗衣液，助力合作伙伴以更绿色的产品开拓中高端洗衣液市场。面对人口不断增长致使粮食与食品需求激增的现状，诺维信积极研发并与合作伙伴达成农业联盟，用生物技术克服现行化学肥料和化学农药对生态环境的污染，同时降低成本、改善农作物品质等使种植业步入良态循环，长效增产。今天人们正孜孜不倦地寻求可再生能源的替代能源，由诺维信最新推出的Eversa®，是市场上第一个利用废油来生产生物柴油的酶制剂解决方案。与此同时，诺维信的Cellic® 作为纤维素乙醇产生过程中必不可少的催化剂，它的问世让农业废弃物从环境、大气污染源之一，变成输送未来清洁能源的原料。到2020年，诺维信全球还计划推出10项改变生活的革命性创新产品，实现二氧化碳减排1亿吨的重大目标。诺维信的愿景就是在更繁荣的经济，更清洁的能源和更美好的生活之间实现和谐与统一。长按下方二维码，选择“识别图中二维码”，了解诺维信中国运营业务，领略生物技术的魅力，更多礼品等待您。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -924,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1272,7 +1274,7 @@
         <v>65</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>66</v>
@@ -1300,7 +1302,7 @@
         <v>70</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>71</v>
@@ -1495,11 +1497,11 @@
       <c r="B41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>115</v>
+      <c r="C41" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>116</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1507,13 +1509,13 @@
         <v>42195.926215277781</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1521,13 +1523,13 @@
         <v>42168.950532407405</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1535,13 +1537,13 @@
         <v>42166.710879629631</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1549,13 +1551,13 @@
         <v>42164.710648148146</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1563,13 +1565,13 @@
         <v>42160.940150462964</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1577,13 +1579,13 @@
         <v>42136.496851851851</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1591,13 +1593,13 @@
         <v>42129.774351851855</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1605,13 +1607,13 @@
         <v>42118.920891203707</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1619,13 +1621,13 @@
         <v>42116.922615740739</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1633,13 +1635,13 @@
         <v>42107.623611111114</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1647,13 +1649,13 @@
         <v>42099.50236111111</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1661,13 +1663,13 @@
         <v>42084.700995370367</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1675,13 +1677,13 @@
         <v>42071.582569444443</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1689,13 +1691,13 @@
         <v>42060.581724537034</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1703,13 +1705,13 @@
         <v>42059.449050925927</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1717,13 +1719,13 @@
         <v>42051.714143518519</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1732,8 +1734,9 @@
     <hyperlink ref="C35" r:id="rId1" location="rd"/>
     <hyperlink ref="C27" r:id="rId2" location="rd"/>
     <hyperlink ref="C25" r:id="rId3" location="rd"/>
+    <hyperlink ref="C41" r:id="rId4" location="rd"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>